<commit_message>
Fix: Correct default plugin namespace; split namespace and keys with ':'
</commit_message>
<xml_diff>
--- a/src/integration-test/resources/simpleImportComplexMetadata.simple.xlsx
+++ b/src/integration-test/resources/simpleImportComplexMetadata.simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adjl/code/maurodatamapper-plugins/mdm-plugin-excel/src/integration-test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688C7135-8205-3847-81FF-7DBAA341A8C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4CD6CF-8B31-3A4A-ACFD-1F178BEBC926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataModels" sheetId="1" r:id="rId1"/>
@@ -197,15 +197,6 @@
     <t>some extra info</t>
   </si>
   <si>
-    <t>uk.ac.ox.softeng.maurodatamapper.plugins.excel:reviewed</t>
-  </si>
-  <si>
-    <t>uk.ac.ox.softeng.maurodatamapper.plugins.excel:approved</t>
-  </si>
-  <si>
-    <t>uk.ac.ox.softeng.maurodatamapper.plugins.excel:distributed</t>
-  </si>
-  <si>
     <t>uk.ac.ox.softeng.maurodatamapper.plugins.database:dialect</t>
   </si>
   <si>
@@ -228,6 +219,15 @@
   </si>
   <si>
     <t>uk.ac.ox.softeng.maurodatamapper.test:blob</t>
+  </si>
+  <si>
+    <t>uk.ac.ox.softeng.maurodatamapper.plugins.excel.simple:reviewed</t>
+  </si>
+  <si>
+    <t>uk.ac.ox.softeng.maurodatamapper.plugins.excel.simple:approved</t>
+  </si>
+  <si>
+    <t>uk.ac.ox.softeng.maurodatamapper.plugins.excel.simple:distributed</t>
   </si>
 </sst>
 </file>
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -628,8 +628,8 @@
     <col min="3" max="4" width="25.83203125" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="25.83203125" customWidth="1"/>
-    <col min="7" max="8" width="48.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="54" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -653,16 +653,16 @@
         <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -820,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -868,16 +868,16 @@
         <v>55</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -893,7 +893,7 @@
       <c r="I2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -996,7 +996,7 @@
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1021,7 +1021,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="L7" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M7" s="6"/>
     </row>
@@ -1049,7 +1049,7 @@
         <v>26</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M8" s="6"/>
     </row>

</xml_diff>